<commit_message>
WIP: code not finished
</commit_message>
<xml_diff>
--- a/hotels_list.xlsx
+++ b/hotels_list.xlsx
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hôtel Avenir Jonquière</t>
+          <t>APA Hotel Asakusa Ekimae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,25 +473,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Scored 7.8</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Good
-2,415 reviews</t>
+          <t>Very Good
+5,474 reviews</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4.5 km from downtown</t>
+          <t>50 m from center</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HOTEL DU PRINTEMPS</t>
+          <t>APA Hotel Roppongi SIX</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,25 +501,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Scored 8.1</t>
+          <t>Scored 7.9</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Very Good
-2,973 reviews</t>
+          <t>Good
+10,789 reviews</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2.7 km from downtown</t>
+          <t>2.3 km from center</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hotel de l'Europe</t>
+          <t>APA Hotel Higashi Shinjuku Kabukicho Tower</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -529,25 +529,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Scored 7.1</t>
+          <t>Scored 8.1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Good
-2,844 reviews</t>
+          <t>Very Good
+19,368 reviews</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3.8 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hotel Marena</t>
+          <t>THE TOURIST HOTEL &amp; Cafe AKIHABARA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -557,25 +557,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Scored 8.4</t>
+          <t>Scored 8.7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Very Good
-1,864 reviews</t>
+          <t>Excellent
+4,320 reviews</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2.6 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hotel Terminus Montparnasse</t>
+          <t>APA Hotel PRIDE Akasaka Kokkaigijidomae</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -585,25 +585,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Scored 7.3</t>
+          <t>Scored 8.4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Good
-3,578 reviews</t>
+          <t>Very Good
+8,157 reviews</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.5 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Le Hameau de Passy</t>
+          <t>APA Hotel &amp; Resort Ryogoku Eki Tower</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -613,25 +613,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Scored 7.7</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Good
-2,809 reviews</t>
+          <t>Very Good
+15,060 reviews</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5.3 km from downtown</t>
+          <t>6 km from center</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Courcelles Etoile</t>
+          <t>Best Western Hotel Fino Tokyo Akihabara</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -641,25 +641,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Scored 8.3</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>Very Good
-1,940 reviews</t>
+3,281 reviews</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hôtel Avama Prony</t>
+          <t>Asakusa Ryokan Toukaisou</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -669,25 +669,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Scored 7.5</t>
+          <t>Scored 8.9</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Good
-984 reviews</t>
+          <t>Excellent
+1,038 reviews</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chatillon Paris Montparnasse</t>
+          <t>THE KNOT TOKYO Shinjuku</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -697,25 +697,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Scored 8.4</t>
+          <t>Scored 8.3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Very Good
-1,556 reviews</t>
+10,518 reviews</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hotel de Neuville Arc de Triomphe</t>
+          <t>Hotel Nihonbashi Saibo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -725,25 +725,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Scored 8.2</t>
+          <t>Scored 8.5</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Very Good
-821 reviews</t>
+2,934 reviews</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5 km from downtown</t>
+          <t>250 m from center</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Studio de charme centre paris 10 min de république</t>
+          <t>Tabist Urban Stays Asakusa</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -753,25 +753,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Scored 8.6</t>
+          <t>Scored 8.0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Excellent
-22 reviews</t>
+          <t>Very Good
+1,642 reviews</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2.6 km from downtown</t>
+          <t>350 m from center</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hôtel de la Terrasse</t>
+          <t>LANDABOUT TOKYO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -781,25 +781,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Scored 6.8</t>
+          <t>Scored 8.7</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Review score
-765 reviews</t>
+          <t>Excellent
+3,627 reviews</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.5 km from downtown</t>
+          <t>6.1 km from center</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hôtel Diva Opera</t>
+          <t>Restay Frontier (Adult Only)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -809,25 +809,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Scored 8.0</t>
+          <t>Scored 8.7</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Very Good
-1,739 reviews</t>
+          <t>Excellent
+621 reviews</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.9 km from downtown</t>
+          <t>3.3 km from center</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hôtel de Bordeaux</t>
+          <t>Akabane Holic Hotel</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -837,25 +837,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Scored 7.5</t>
+          <t>Scored 8.5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Good
-2,996 reviews</t>
+          <t>Very Good
+3,967 reviews</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2 km from downtown</t>
+          <t>8 km from center</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hilton Garden Inn Paris La Villette</t>
+          <t>Toshi Center Hotel</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -865,25 +865,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Scored 8.7</t>
+          <t>Scored 8.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Excellent
-571 reviews</t>
+          <t>Very Good
+3,826 reviews</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Prince Monceau</t>
+          <t>HOTEL MYSTAYS Asakusabashi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -893,25 +893,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Scored 7.0</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Good
-1,672 reviews</t>
+          <t>Very Good
+2,403 reviews</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4.4 km from downtown</t>
+          <t>300 m from center</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hotel Cactus</t>
+          <t>Forest Hongo by unito</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -921,25 +921,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Scored 7.2</t>
+          <t>Scored 8.6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Good
-2,171 reviews</t>
+          <t>Excellent
+1,018 reviews</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3.6 km from downtown</t>
+          <t>0.5 km from center</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hotel des Belges</t>
+          <t>SF Heigths</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -949,25 +949,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Scored 7.4</t>
+          <t>Scored 7.3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>Good
-1,327 reviews</t>
+15 reviews</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.5 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Montparnasse Daguerre</t>
+          <t>APA Hotel Nihombashi Bakuroyokoyama Ekimae</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -977,25 +977,25 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Scored 8.2</t>
+          <t>Scored 8.4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>Very Good
-2,393 reviews</t>
+4,241 reviews</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3 km from downtown</t>
+          <t>0.6 km from center</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hotel London</t>
+          <t>APA Hotel Asakusa Kuramae Kita</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1005,25 +1005,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Scored 8.2</t>
+          <t>Scored 8.5</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>Very Good
-2,109 reviews</t>
+5,064 reviews</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2 km from downtown</t>
+          <t>350 m from center</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hôtel Aston Paris</t>
+          <t>Hotel Asakusa KANNONURA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1033,25 +1033,25 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Scored 7.7</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Good
-2,476 reviews</t>
+          <t>Very Good
+853 reviews</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.8 km from downtown</t>
+          <t>center</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kyriad Paris 10 - Canal Saint Martin - République</t>
+          <t>APA Hotel TKP Nippori Ekimae</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1061,25 +1061,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Scored 7.7</t>
+          <t>Scored 8.1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Good
-615 reviews</t>
+          <t>Very Good
+2,097 reviews</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.9 km from downtown</t>
+          <t>0.9 km from center</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hôtel Central Bastille</t>
+          <t>NEW OPEN!! RUTiLE IKEBUKURO TOKYO</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1089,25 +1089,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Scored 6.2</t>
+          <t>Scored 8.6</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Review score
-862 reviews</t>
+          <t>Excellent
+20 reviews</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.5 km from downtown</t>
+          <t>4.1 km from center</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Le Lampika Hôtel</t>
+          <t>ART HOTELS SHIBUYA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1117,25 +1117,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Scored 8.5</t>
+          <t>Scored 8.6</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Very Good
-388 reviews</t>
+          <t>Excellent
+1,154 reviews</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3 km from downtown</t>
+          <t>250 m from center</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HotelF1 Paris Saint Ouen Marché Aux Puces</t>
+          <t>HOTEL TAVINOS Hamamatsucho</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1145,18 +1145,18 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Scored 6.7</t>
+          <t>Scored 8.2</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Review score
-18,493 reviews</t>
+          <t>Very Good
+1,191 reviews</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5.1 km from downtown</t>
+          <t>200 m from center</t>
         </is>
       </c>
     </row>

</xml_diff>